<commit_message>
Foot in the door exclamation mark
</commit_message>
<xml_diff>
--- a/inputs_for_prioritization_model.xlsx
+++ b/inputs_for_prioritization_model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\ais_prioritization_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\SAR_prioritization_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C17CDBE-4020-49D8-8512-0F250B6792C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBFC1EE-7D11-4C58-A006-DE1DAED1554E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{EB2B9178-B69B-457E-8E21-B51FD6DB9907}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
   <si>
     <t>Region</t>
   </si>
@@ -414,9 +414,6 @@
   </si>
   <si>
     <t>Fraser River Watershed</t>
-  </si>
-  <si>
-    <t>Smallmouth bass, Goldfish, Pumpkinseed, Largemouth bass, Yellow perch, Asian clam, Northern pike, Common carp, Brown bullhead</t>
   </si>
 </sst>
 </file>
@@ -803,7 +800,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +832,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>122</v>
@@ -850,7 +847,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
         <v>124</v>

</xml_diff>